<commit_message>
Added Techs in the excel file and import
</commit_message>
<xml_diff>
--- a/civilization-rest/src/main/resources/assets/gamedata-faf-waw.xlsx
+++ b/civilization-rest/src/main/resources/assets/gamedata-faf-waw.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" activeTab="13"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" firstSheet="3" activeTab="17"/>
   </bookViews>
   <sheets>
     <sheet name="Civ" sheetId="1" r:id="rId1"/>
@@ -18,16 +18,20 @@
     <sheet name="Aircraft" sheetId="10" r:id="rId9"/>
     <sheet name="Villages" sheetId="16" r:id="rId10"/>
     <sheet name="Huts" sheetId="12" r:id="rId11"/>
-    <sheet name="Wonders " sheetId="13" r:id="rId12"/>
+    <sheet name="Wonders" sheetId="13" r:id="rId12"/>
     <sheet name="Tiles" sheetId="14" r:id="rId13"/>
     <sheet name="City-states" sheetId="15" r:id="rId14"/>
+    <sheet name="Level 1 Tech" sheetId="17" r:id="rId15"/>
+    <sheet name="Level 2 Tech" sheetId="18" r:id="rId16"/>
+    <sheet name="Level 3 Tech" sheetId="19" r:id="rId17"/>
+    <sheet name="Level 4 Tech" sheetId="20" r:id="rId18"/>
   </sheets>
   <calcPr calcId="145621" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="347">
   <si>
     <t>Civilization</t>
   </si>
@@ -936,13 +940,148 @@
   </si>
   <si>
     <t>1 Random Resource &amp; 1 Hammer &amp; 1 Trade.</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Animal Husbandry</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Code of Laws</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Horseback Riding</t>
+  </si>
+  <si>
+    <t>Masonry</t>
+  </si>
+  <si>
+    <t>Metalworking</t>
+  </si>
+  <si>
+    <t>Navigation</t>
+  </si>
+  <si>
+    <t>Philosophy</t>
+  </si>
+  <si>
+    <t>Pottery</t>
+  </si>
+  <si>
+    <t>Writing</t>
+  </si>
+  <si>
+    <t>Navy</t>
+  </si>
+  <si>
+    <t>Civil Service</t>
+  </si>
+  <si>
+    <t>Chivalry</t>
+  </si>
+  <si>
+    <t>Construction</t>
+  </si>
+  <si>
+    <t>Democracy</t>
+  </si>
+  <si>
+    <t>Engineering</t>
+  </si>
+  <si>
+    <t>Irrigation</t>
+  </si>
+  <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
+    <t>Monarchy</t>
+  </si>
+  <si>
+    <t>Mysticism</t>
+  </si>
+  <si>
+    <t>Printing Press</t>
+  </si>
+  <si>
+    <t>Sailing</t>
+  </si>
+  <si>
+    <t>Logistics</t>
+  </si>
+  <si>
+    <t>Bureaucracy</t>
+  </si>
+  <si>
+    <t>Banking</t>
+  </si>
+  <si>
+    <t>Biology</t>
+  </si>
+  <si>
+    <t>Communism</t>
+  </si>
+  <si>
+    <t>Ecology</t>
+  </si>
+  <si>
+    <t>Gunpowder</t>
+  </si>
+  <si>
+    <t>Metal Casting</t>
+  </si>
+  <si>
+    <t>Military Science</t>
+  </si>
+  <si>
+    <t>Railroad</t>
+  </si>
+  <si>
+    <t>Steam Power</t>
+  </si>
+  <si>
+    <t>Theology</t>
+  </si>
+  <si>
+    <t>Education</t>
+  </si>
+  <si>
+    <t>Atomic Theory</t>
+  </si>
+  <si>
+    <t>Ballistics</t>
+  </si>
+  <si>
+    <t>Combustion</t>
+  </si>
+  <si>
+    <t>Computers</t>
+  </si>
+  <si>
+    <t>Flight</t>
+  </si>
+  <si>
+    <t>Mass Media</t>
+  </si>
+  <si>
+    <t>Plastics</t>
+  </si>
+  <si>
+    <t>Replacement Parts</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -957,6 +1096,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -979,7 +1125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -996,6 +1142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2449,7 +2596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
@@ -2475,7 +2622,7 @@
       </c>
       <c r="B2" s="2">
         <f ca="1">RAND()</f>
-        <v>0.63067811233014115</v>
+        <v>0.53743030962215166</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2484,7 +2631,7 @@
       </c>
       <c r="B3" s="2">
         <f ca="1">RAND()</f>
-        <v>0.55210034023805887</v>
+        <v>0.90359721286465877</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -2493,7 +2640,7 @@
       </c>
       <c r="B4" s="2">
         <f ca="1">RAND()</f>
-        <v>5.3011397440666852E-2</v>
+        <v>0.21140014064583623</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -2502,7 +2649,7 @@
       </c>
       <c r="B5" s="2">
         <f ca="1">RAND()</f>
-        <v>0.43511889523821967</v>
+        <v>0.94813315548976063</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -2511,12 +2658,342 @@
       </c>
       <c r="B6" s="2">
         <f ca="1">RAND()</f>
-        <v>0.34599895173895823</v>
+        <v>0.40849917523548063</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>327</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>338</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M47" sqref="M47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>302</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>345</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added trading. Added Starting tech when choosing civilization. Started work on techtree. Fixed Chat
</commit_message>
<xml_diff>
--- a/civilization-rest/src/main/resources/assets/gamedata-faf-waw.xlsx
+++ b/civilization-rest/src/main/resources/assets/gamedata-faf-waw.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Civ" sheetId="1" state="visible" r:id="rId2"/>
@@ -32,57 +32,108 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="531" uniqueCount="352">
   <si>
     <t>Civilization</t>
   </si>
   <si>
+    <t>Starting Tech</t>
+  </si>
+  <si>
     <t>Americans</t>
   </si>
   <si>
+    <t>Currency</t>
+  </si>
+  <si>
     <t>Arabs</t>
   </si>
   <si>
+    <t>Mathematics</t>
+  </si>
+  <si>
     <t>Aztecs</t>
   </si>
   <si>
+    <t>Irrigation</t>
+  </si>
+  <si>
     <t>Chinese</t>
   </si>
   <si>
+    <t>Writing</t>
+  </si>
+  <si>
     <t>Egyptians</t>
   </si>
   <si>
+    <t>Construction</t>
+  </si>
+  <si>
     <t>England</t>
   </si>
   <si>
+    <t>Navy</t>
+  </si>
+  <si>
     <t>French</t>
   </si>
   <si>
+    <t>Pottery</t>
+  </si>
+  <si>
     <t>Germans</t>
   </si>
   <si>
+    <t>Metalworking</t>
+  </si>
+  <si>
     <t>Greeks</t>
   </si>
   <si>
+    <t>Democracy</t>
+  </si>
+  <si>
     <t>Indians</t>
   </si>
   <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
     <t>Japanese</t>
   </si>
   <si>
+    <t>Chivalry</t>
+  </si>
+  <si>
     <t>Mongols</t>
   </si>
   <si>
+    <t>Horseback Riding</t>
+  </si>
+  <si>
     <t>Romans</t>
   </si>
   <si>
+    <t>Code of Laws</t>
+  </si>
+  <si>
     <t>Russians</t>
   </si>
   <si>
+    <t>Communism</t>
+  </si>
+  <si>
     <t>Spanish</t>
   </si>
   <si>
+    <t>Navigation</t>
+  </si>
+  <si>
     <t>Zulu</t>
+  </si>
+  <si>
+    <t>Animal Husbandry</t>
   </si>
   <si>
     <t>Card Name</t>
@@ -958,63 +1009,18 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Animal Husbandry</t>
-  </si>
-  <si>
-    <t>Agriculture</t>
-  </si>
-  <si>
-    <t>Code of Laws</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Horseback Riding</t>
-  </si>
-  <si>
     <t>Masonry</t>
   </si>
   <si>
-    <t>Metalworking</t>
-  </si>
-  <si>
-    <t>Navigation</t>
-  </si>
-  <si>
     <t>Philosophy</t>
   </si>
   <si>
-    <t>Pottery</t>
-  </si>
-  <si>
-    <t>Writing</t>
-  </si>
-  <si>
-    <t>Navy</t>
-  </si>
-  <si>
     <t>Civil Service</t>
   </si>
   <si>
-    <t>Chivalry</t>
-  </si>
-  <si>
-    <t>Construction</t>
-  </si>
-  <si>
-    <t>Democracy</t>
-  </si>
-  <si>
     <t>Engineering</t>
   </si>
   <si>
-    <t>Irrigation</t>
-  </si>
-  <si>
-    <t>Mathematics</t>
-  </si>
-  <si>
     <t>Monarchy</t>
   </si>
   <si>
@@ -1037,9 +1043,6 @@
   </si>
   <si>
     <t>Biology</t>
-  </si>
-  <si>
-    <t>Communism</t>
   </si>
   <si>
     <t>Ecology</t>
@@ -1223,8 +1226,8 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="1" sqref="B2:B6 B19"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1234,90 +1237,140 @@
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>4</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>6</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>8</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>12</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>14</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>22</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>24</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>26</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>28</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>16</v>
+        <v>32</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1339,7 +1392,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="1" sqref="B2:B6 D32"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="1" sqref="B1:B17 D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1350,108 +1403,108 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -1473,7 +1526,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="1" sqref="B2:B6 D20"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="1" sqref="B1:B17 D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1485,183 +1538,183 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="B1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
     </row>
   </sheetData>
@@ -1683,7 +1736,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="1" sqref="B2:B6 G10"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="1" sqref="B1:B17 G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1698,39 +1751,39 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="E1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
       <c r="C2" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>219</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="C3" s="0" t="n">
         <v>15</v>
@@ -1738,10 +1791,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="C4" s="0" t="n">
         <v>10</v>
@@ -1749,123 +1802,123 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="C5" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="C6" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>231</v>
+        <v>248</v>
       </c>
       <c r="C7" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="C8" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="C9" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>238</v>
+        <v>255</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="C10" s="0" t="n">
         <v>15</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="E12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="C13" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="C14" s="0" t="n">
         <v>15</v>
@@ -1873,179 +1926,179 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="C15" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="C16" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="C17" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="C18" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>259</v>
+        <v>276</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="C19" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>264</v>
+        <v>281</v>
       </c>
       <c r="C20" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>265</v>
+        <v>282</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>266</v>
+        <v>283</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>267</v>
+        <v>284</v>
       </c>
       <c r="C21" s="0" t="n">
         <v>20</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="E23" s="1"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>271</v>
+        <v>288</v>
       </c>
       <c r="C24" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>273</v>
+        <v>290</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>274</v>
+        <v>291</v>
       </c>
       <c r="C25" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>275</v>
+        <v>292</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>276</v>
+        <v>293</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>277</v>
+        <v>294</v>
       </c>
       <c r="C26" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>278</v>
+        <v>295</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>279</v>
+        <v>296</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>280</v>
+        <v>297</v>
       </c>
       <c r="C27" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>281</v>
+        <v>298</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>282</v>
+        <v>299</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>283</v>
+        <v>300</v>
       </c>
       <c r="C28" s="0" t="n">
         <v>25</v>
@@ -2053,52 +2106,52 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>284</v>
+        <v>301</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>285</v>
+        <v>302</v>
       </c>
       <c r="C29" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>286</v>
+        <v>303</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>287</v>
+        <v>304</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>288</v>
+        <v>305</v>
       </c>
       <c r="C30" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>289</v>
+        <v>306</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>290</v>
+        <v>307</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>291</v>
+        <v>308</v>
       </c>
       <c r="C31" s="0" t="n">
         <v>25</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>292</v>
+        <v>309</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>293</v>
+        <v>310</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>294</v>
+        <v>311</v>
       </c>
       <c r="C32" s="0" t="n">
         <v>20</v>
@@ -2123,7 +2176,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I31" activeCellId="1" sqref="B2:B6 I31"/>
+      <selection pane="topLeft" activeCell="I31" activeCellId="1" sqref="B1:B17 I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2134,7 +2187,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="B1" s="1"/>
     </row>
@@ -2291,8 +2344,8 @@
   </sheetPr>
   <dimension ref="A1:B16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2305,50 +2358,50 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>295</v>
+        <v>312</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>296</v>
+        <v>313</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>297</v>
+        <v>314</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>298</v>
+        <v>315</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>299</v>
+        <v>316</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>301</v>
+        <v>318</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>302</v>
+        <v>319</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>303</v>
+        <v>320</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>304</v>
+        <v>321</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>305</v>
+        <v>322</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2375,7 +2428,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="B2:B6 D18"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="B1:B17 D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2386,70 +2439,70 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>307</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>308</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>309</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>310</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>311</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>313</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>314</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>315</v>
+        <v>325</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>316</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>317</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>318</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2471,7 +2524,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B2:B6 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B1:B17 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2482,75 +2535,75 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>320</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>321</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>322</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>324</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>325</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -2572,7 +2625,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="B2:B6 B8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B1:B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2583,65 +2636,65 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>334</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -2663,7 +2716,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M47" activeCellId="1" sqref="B2:B6 M47"/>
+      <selection pane="topLeft" activeCell="M47" activeCellId="1" sqref="B1:B17 M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2674,55 +2727,55 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>306</v>
+        <v>323</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -2744,7 +2797,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="B2:B6 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="B1:B17 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2756,253 +2809,253 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>25</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>36</v>
+        <v>53</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>38</v>
+        <v>55</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>44</v>
+        <v>61</v>
       </c>
       <c r="C28" s="2"/>
     </row>
@@ -3025,7 +3078,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="B2:B6 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="B1:B17 C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3037,235 +3090,235 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>64</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>49</v>
+        <v>66</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>51</v>
+        <v>68</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>52</v>
+        <v>69</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>54</v>
+        <v>71</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
       <c r="C19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="C22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
       <c r="C23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>42</v>
+        <v>59</v>
       </c>
       <c r="C24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -3288,7 +3341,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="1" sqref="B2:B6 A14"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="1" sqref="B1:B17 A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3300,163 +3353,163 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="C1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>71</v>
+        <v>88</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>73</v>
+        <v>90</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>74</v>
+        <v>91</v>
       </c>
       <c r="C4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>76</v>
+        <v>93</v>
       </c>
       <c r="C5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>77</v>
+        <v>94</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>78</v>
+        <v>95</v>
       </c>
       <c r="C7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>80</v>
+        <v>97</v>
       </c>
       <c r="C8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>81</v>
+        <v>98</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="C9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="C11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="C13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="C15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="C16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="C17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="C18" s="2"/>
     </row>
@@ -3479,7 +3532,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="1" sqref="B2:B6 C46"/>
+      <selection pane="topLeft" activeCell="C46" activeCellId="1" sqref="B1:B17 C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3493,517 +3546,517 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="D1" s="3"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="D2" s="4"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>98</v>
+        <v>115</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>100</v>
+        <v>117</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>101</v>
+        <v>118</v>
       </c>
       <c r="D4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>103</v>
+        <v>120</v>
       </c>
       <c r="D5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>104</v>
+        <v>121</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>105</v>
+        <v>122</v>
       </c>
       <c r="D6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="D7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>109</v>
+        <v>126</v>
       </c>
       <c r="D8" s="4"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="D9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="D10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="D11" s="4"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="D12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="D13" s="4"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>121</v>
+        <v>138</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="D14" s="4"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>123</v>
+        <v>140</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>124</v>
+        <v>141</v>
       </c>
       <c r="D15" s="4"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
-        <v>125</v>
+        <v>142</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>127</v>
+        <v>144</v>
       </c>
       <c r="D16" s="4"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
-        <v>128</v>
+        <v>145</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>129</v>
+        <v>146</v>
       </c>
       <c r="D17" s="4"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>130</v>
+        <v>147</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>132</v>
+        <v>149</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>133</v>
+        <v>150</v>
       </c>
       <c r="D19" s="4"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>134</v>
+        <v>151</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="D20" s="4"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>136</v>
+        <v>153</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>137</v>
+        <v>154</v>
       </c>
       <c r="D21" s="4"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>138</v>
+        <v>155</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>126</v>
+        <v>143</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>139</v>
+        <v>156</v>
       </c>
       <c r="D22" s="4"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>142</v>
+        <v>159</v>
       </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>143</v>
+        <v>160</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>144</v>
+        <v>161</v>
       </c>
       <c r="D24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="4" t="s">
-        <v>145</v>
+        <v>162</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>146</v>
+        <v>163</v>
       </c>
       <c r="D25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>147</v>
+        <v>164</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>148</v>
+        <v>165</v>
       </c>
       <c r="D26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="D27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="4" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>152</v>
+        <v>169</v>
       </c>
       <c r="D28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>141</v>
+        <v>158</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="D29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
       <c r="D30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>158</v>
+        <v>175</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="D31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="D32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="D33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="D34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="D35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="D36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="D37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="D38" s="4"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="D39" s="4"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="D40" s="4"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>179</v>
+        <v>196</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="D41" s="4"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="D42" s="4"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="D43" s="4"/>
     </row>
@@ -4026,7 +4079,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="1" sqref="B2:B6 D21"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="1" sqref="B1:B17 D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4040,16 +4093,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -4282,7 +4335,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="B2:B6 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="B1:B17 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4293,16 +4346,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -4535,7 +4588,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="B2:B6 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="B1:B17 E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4546,16 +4599,16 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="E1" s="1"/>
     </row>
@@ -4788,7 +4841,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H31" activeCellId="1" sqref="B2:B6 H31"/>
+      <selection pane="topLeft" activeCell="H31" activeCellId="1" sqref="B1:B17 H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4799,7 +4852,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="B1" s="1"/>
     </row>

</xml_diff>

<commit_message>
Deleted images folder and fixed martinluther
</commit_message>
<xml_diff>
--- a/civilization-rest/src/main/resources/assets/gamedata-faf-waw.xlsx
+++ b/civilization-rest/src/main/resources/assets/gamedata-faf-waw.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="600" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Civ" sheetId="1" state="visible" r:id="rId2"/>
@@ -496,7 +496,7 @@
     <t>Leonidas</t>
   </si>
   <si>
-    <t>Battle: Each time you start a battle with fewer units in your battle force than your opponent, your combat bonus is increased by 8 until the end of the battle.</t>
+    <t>Battle: Each time you start a battle as defender with fewer units in your battle force than your opponent, your combat bonus is increased by 8 until the end of the battle.</t>
   </si>
   <si>
     <t>Sun Tzu</t>
@@ -1226,8 +1226,8 @@
   </sheetPr>
   <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1:B17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1392,7 +1392,7 @@
   <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="1" sqref="B1:B17 D32"/>
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1526,7 +1526,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="1" sqref="B1:B17 D20"/>
+      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1736,7 +1736,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="1" sqref="B1:B17 G10"/>
+      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2176,7 +2176,7 @@
   <dimension ref="A1:B28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I31" activeCellId="1" sqref="B1:B17 I31"/>
+      <selection pane="topLeft" activeCell="I31" activeCellId="0" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2345,7 +2345,7 @@
   <dimension ref="A1:B16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B1:B17"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2428,7 +2428,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="1" sqref="B1:B17 D18"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2524,7 +2524,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="B1:B17 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2625,7 +2625,7 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B1:B17"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2716,7 +2716,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M47" activeCellId="1" sqref="B1:B17 M47"/>
+      <selection pane="topLeft" activeCell="M47" activeCellId="0" sqref="M47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2797,7 +2797,7 @@
   <dimension ref="A1:C28"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="B1:B17 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3078,7 +3078,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="1" sqref="B1:B17 C1"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3341,7 +3341,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="1" sqref="B1:B17 A14"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3531,8 +3531,8 @@
   </sheetPr>
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C46" activeCellId="1" sqref="B1:B17 C46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4079,7 +4079,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D21" activeCellId="1" sqref="B1:B17 D21"/>
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4335,7 +4335,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="B1:B17 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4588,7 +4588,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E1" activeCellId="1" sqref="B1:B17 E1"/>
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -4841,7 +4841,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H31" activeCellId="1" sqref="B1:B17 H31"/>
+      <selection pane="topLeft" activeCell="H31" activeCellId="0" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>